<commit_message>
changed example start payroll to company payroll
</commit_message>
<xml_diff>
--- a/docs/PayrollRestServicesEndpoints.xlsx
+++ b/docs/PayrollRestServicesEndpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F908C8BC-FAA9-4457-B3BB-FACE14969730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6404C50-874D-4E5D-A321-4B378FDCBA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoints" sheetId="1" r:id="rId1"/>
@@ -1967,9 +1967,6 @@
     <t>api/</t>
   </si>
   <si>
-    <t>Payroll Engine - REST Service Endpoints</t>
-  </si>
-  <si>
     <t>an: attribute name</t>
   </si>
   <si>
@@ -2022,6 +2019,9 @@
   </si>
   <si>
     <t>Delete calendar</t>
+  </si>
+  <si>
+    <t>Payroll Engine REST Service Endpoints</t>
   </si>
 </sst>
 </file>
@@ -2604,7 +2604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2839,9 +2839,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3194,32 +3191,32 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="1.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="6.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="8.5500000000000007" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
@@ -3237,9 +3234,9 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -3260,7 +3257,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -3278,7 +3275,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
         <v>257</v>
       </c>
@@ -3308,7 +3305,7 @@
       </c>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
         <v>235</v>
       </c>
@@ -3328,7 +3325,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="29" t="s">
         <v>235</v>
       </c>
@@ -3348,7 +3345,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="36" t="s">
         <v>235</v>
       </c>
@@ -3368,7 +3365,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>122</v>
       </c>
@@ -3386,7 +3383,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
         <v>122</v>
       </c>
@@ -3404,7 +3401,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
         <v>122</v>
       </c>
@@ -3424,7 +3421,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
         <v>527</v>
       </c>
@@ -3446,7 +3443,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
         <v>527</v>
       </c>
@@ -3468,7 +3465,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
         <v>527</v>
       </c>
@@ -3476,7 +3473,7 @@
         <v>594</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>183</v>
@@ -3494,7 +3491,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="22" t="s">
         <v>0</v>
       </c>
@@ -3516,7 +3513,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="29" t="s">
         <v>0</v>
       </c>
@@ -3540,7 +3537,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="47" t="s">
         <v>0</v>
       </c>
@@ -3548,7 +3545,7 @@
         <v>172</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E19" s="49" t="s">
         <v>183</v>
@@ -3566,7 +3563,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="29" t="s">
         <v>0</v>
       </c>
@@ -3586,7 +3583,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="29" t="s">
         <v>0</v>
       </c>
@@ -3606,7 +3603,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36" t="s">
         <v>0</v>
       </c>
@@ -3626,58 +3623,58 @@
       <c r="J22" s="5"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>619</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>620</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="24" t="s">
+        <v>624</v>
+      </c>
+      <c r="F23" s="43" t="s">
         <v>625</v>
       </c>
-      <c r="F23" s="43" t="s">
-        <v>626</v>
-      </c>
       <c r="G23" s="26" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="26"/>
       <c r="J23" s="5"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="29" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G24" s="33"/>
       <c r="H24" s="34" t="s">
+        <v>628</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>629</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>630</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="9"/>
     </row>
-    <row r="25" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="47" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="49" t="s">
@@ -3686,18 +3683,18 @@
       <c r="F25" s="54" t="s">
         <v>354</v>
       </c>
-      <c r="G25" s="79"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="52"/>
       <c r="I25" s="51"/>
       <c r="J25" s="5"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="47" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="49" t="s">
@@ -3706,18 +3703,18 @@
       <c r="F26" s="54" t="s">
         <v>357</v>
       </c>
-      <c r="G26" s="79"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="52"/>
       <c r="I26" s="51"/>
       <c r="J26" s="5"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="47" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D27" s="48"/>
       <c r="E27" s="49" t="s">
@@ -3726,13 +3723,13 @@
       <c r="F27" s="54" t="s">
         <v>355</v>
       </c>
-      <c r="G27" s="79"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="52"/>
       <c r="I27" s="51"/>
       <c r="J27" s="5"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="22" t="s">
         <v>37</v>
       </c>
@@ -3756,7 +3753,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="29" t="s">
         <v>37</v>
       </c>
@@ -3780,7 +3777,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="29" t="s">
         <v>37</v>
       </c>
@@ -3802,7 +3799,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="56" t="s">
         <v>37</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>173</v>
       </c>
       <c r="D31" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E31" s="58" t="s">
         <v>183</v>
@@ -3828,7 +3825,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="22" t="s">
         <v>186</v>
       </c>
@@ -3850,7 +3847,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="29" t="s">
         <v>186</v>
       </c>
@@ -3874,7 +3871,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="56" t="s">
         <v>186</v>
       </c>
@@ -3882,7 +3879,7 @@
         <v>535</v>
       </c>
       <c r="D34" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>183</v>
@@ -3900,7 +3897,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>460</v>
       </c>
@@ -3922,7 +3919,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="29" t="s">
         <v>460</v>
       </c>
@@ -3946,7 +3943,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="56" t="s">
         <v>460</v>
       </c>
@@ -3954,7 +3951,7 @@
         <v>539</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E37" s="58" t="s">
         <v>183</v>
@@ -3972,7 +3969,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="22" t="s">
         <v>507</v>
       </c>
@@ -3994,7 +3991,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="29" t="s">
         <v>507</v>
       </c>
@@ -4016,7 +4013,7 @@
       <c r="J39" s="5"/>
       <c r="K39" s="9"/>
     </row>
-    <row r="40" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="29" t="s">
         <v>507</v>
       </c>
@@ -4038,7 +4035,7 @@
       <c r="J40" s="5"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="36" t="s">
         <v>507</v>
       </c>
@@ -4060,7 +4057,7 @@
       <c r="J41" s="5"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="22" t="s">
         <v>476</v>
       </c>
@@ -4082,7 +4079,7 @@
       <c r="J42" s="5"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="29" t="s">
         <v>476</v>
       </c>
@@ -4102,7 +4099,7 @@
       <c r="J43" s="5"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="29" t="s">
         <v>476</v>
       </c>
@@ -4122,7 +4119,7 @@
       <c r="J44" s="5"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="29" t="s">
         <v>476</v>
       </c>
@@ -4142,7 +4139,7 @@
       <c r="J45" s="5"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="29" t="s">
         <v>476</v>
       </c>
@@ -4162,7 +4159,7 @@
       <c r="J46" s="5"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="29" t="s">
         <v>476</v>
       </c>
@@ -4184,7 +4181,7 @@
       <c r="J47" s="5"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="29" t="s">
         <v>476</v>
       </c>
@@ -4206,7 +4203,7 @@
       <c r="J48" s="5"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="36" t="s">
         <v>476</v>
       </c>
@@ -4226,7 +4223,7 @@
       <c r="J49" s="5"/>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="22" t="s">
         <v>477</v>
       </c>
@@ -4248,7 +4245,7 @@
       <c r="J50" s="5"/>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="29" t="s">
         <v>477</v>
       </c>
@@ -4268,7 +4265,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="29" t="s">
         <v>477</v>
       </c>
@@ -4288,7 +4285,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="29" t="s">
         <v>477</v>
       </c>
@@ -4308,7 +4305,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="29" t="s">
         <v>477</v>
       </c>
@@ -4328,7 +4325,7 @@
       <c r="J54" s="5"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="29" t="s">
         <v>477</v>
       </c>
@@ -4350,7 +4347,7 @@
       <c r="J55" s="5"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="29" t="s">
         <v>477</v>
       </c>
@@ -4372,7 +4369,7 @@
       <c r="J56" s="5"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="36" t="s">
         <v>477</v>
       </c>
@@ -4392,7 +4389,7 @@
       <c r="J57" s="5"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="22" t="s">
         <v>5</v>
       </c>
@@ -4414,7 +4411,7 @@
       <c r="J58" s="5"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="29" t="s">
         <v>5</v>
       </c>
@@ -4434,7 +4431,7 @@
       <c r="J59" s="5"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="29" t="s">
         <v>5</v>
       </c>
@@ -4454,7 +4451,7 @@
       <c r="J60" s="5"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="29" t="s">
         <v>5</v>
       </c>
@@ -4474,7 +4471,7 @@
       <c r="J61" s="5"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="29" t="s">
         <v>5</v>
       </c>
@@ -4494,7 +4491,7 @@
       <c r="J62" s="5"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="29" t="s">
         <v>5</v>
       </c>
@@ -4516,7 +4513,7 @@
       <c r="J63" s="5"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="29" t="s">
         <v>5</v>
       </c>
@@ -4538,7 +4535,7 @@
       <c r="J64" s="5"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="36" t="s">
         <v>5</v>
       </c>
@@ -4558,7 +4555,7 @@
       <c r="J65" s="5"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="22" t="s">
         <v>6</v>
       </c>
@@ -4580,7 +4577,7 @@
       <c r="J66" s="5"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="29" t="s">
         <v>6</v>
       </c>
@@ -4604,7 +4601,7 @@
       <c r="J67" s="5"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="29" t="s">
         <v>6</v>
       </c>
@@ -4612,7 +4609,7 @@
         <v>174</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E68" s="49" t="s">
         <v>183</v>
@@ -4630,7 +4627,7 @@
       <c r="J68" s="5"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="29" t="s">
         <v>6</v>
       </c>
@@ -4652,7 +4649,7 @@
       <c r="J69" s="5"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="29" t="s">
         <v>6</v>
       </c>
@@ -4672,7 +4669,7 @@
       <c r="J70" s="5"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="29" t="s">
         <v>6</v>
       </c>
@@ -4692,7 +4689,7 @@
       <c r="J71" s="5"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="72" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="29" t="s">
         <v>6</v>
       </c>
@@ -4712,7 +4709,7 @@
       <c r="J72" s="5"/>
       <c r="K72" s="9"/>
     </row>
-    <row r="73" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="29" t="s">
         <v>6</v>
       </c>
@@ -4732,7 +4729,7 @@
       <c r="J73" s="5"/>
       <c r="K73" s="9"/>
     </row>
-    <row r="74" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="29" t="s">
         <v>6</v>
       </c>
@@ -4754,7 +4751,7 @@
       <c r="J74" s="5"/>
       <c r="K74" s="9"/>
     </row>
-    <row r="75" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="29" t="s">
         <v>6</v>
       </c>
@@ -4776,7 +4773,7 @@
       <c r="J75" s="5"/>
       <c r="K75" s="9"/>
     </row>
-    <row r="76" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="36" t="s">
         <v>6</v>
       </c>
@@ -4796,7 +4793,7 @@
       <c r="J76" s="5"/>
       <c r="K76" s="9"/>
     </row>
-    <row r="77" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
         <v>193</v>
       </c>
@@ -4818,7 +4815,7 @@
       <c r="J77" s="5"/>
       <c r="K77" s="9"/>
     </row>
-    <row r="78" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="29" t="s">
         <v>193</v>
       </c>
@@ -4826,7 +4823,7 @@
         <v>359</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E78" s="31" t="s">
         <v>190</v>
@@ -4840,7 +4837,7 @@
       <c r="J78" s="5"/>
       <c r="K78" s="9"/>
     </row>
-    <row r="79" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="29" t="s">
         <v>193</v>
       </c>
@@ -4864,7 +4861,7 @@
       <c r="J79" s="5"/>
       <c r="K79" s="9"/>
     </row>
-    <row r="80" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="29" t="s">
         <v>193</v>
       </c>
@@ -4872,7 +4869,7 @@
         <v>543</v>
       </c>
       <c r="D80" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E80" s="49" t="s">
         <v>183</v>
@@ -4890,7 +4887,7 @@
       <c r="J80" s="5"/>
       <c r="K80" s="9"/>
     </row>
-    <row r="81" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="29" t="s">
         <v>193</v>
       </c>
@@ -4912,7 +4909,7 @@
       <c r="J81" s="5"/>
       <c r="K81" s="9"/>
     </row>
-    <row r="82" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="29" t="s">
         <v>193</v>
       </c>
@@ -4936,7 +4933,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="9"/>
     </row>
-    <row r="83" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="29" t="s">
         <v>193</v>
       </c>
@@ -4954,7 +4951,7 @@
       <c r="J83" s="5"/>
       <c r="K83" s="9"/>
     </row>
-    <row r="84" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="29" t="s">
         <v>193</v>
       </c>
@@ -4976,7 +4973,7 @@
       <c r="J84" s="5"/>
       <c r="K84" s="9"/>
     </row>
-    <row r="85" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="29" t="s">
         <v>193</v>
       </c>
@@ -5000,7 +4997,7 @@
       <c r="J85" s="5"/>
       <c r="K85" s="9"/>
     </row>
-    <row r="86" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="29" t="s">
         <v>193</v>
       </c>
@@ -5022,7 +5019,7 @@
       <c r="J86" s="5"/>
       <c r="K86" s="9"/>
     </row>
-    <row r="87" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="29" t="s">
         <v>193</v>
       </c>
@@ -5046,7 +5043,7 @@
       <c r="J87" s="5"/>
       <c r="K87" s="9"/>
     </row>
-    <row r="88" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="29" t="s">
         <v>193</v>
       </c>
@@ -5068,7 +5065,7 @@
       <c r="J88" s="5"/>
       <c r="K88" s="9"/>
     </row>
-    <row r="89" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="29" t="s">
         <v>193</v>
       </c>
@@ -5092,7 +5089,7 @@
       <c r="J89" s="5"/>
       <c r="K89" s="9"/>
     </row>
-    <row r="90" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="29" t="s">
         <v>193</v>
       </c>
@@ -5114,7 +5111,7 @@
       <c r="J90" s="5"/>
       <c r="K90" s="9"/>
     </row>
-    <row r="91" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="29" t="s">
         <v>193</v>
       </c>
@@ -5138,7 +5135,7 @@
       <c r="J91" s="5"/>
       <c r="K91" s="9"/>
     </row>
-    <row r="92" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="29" t="s">
         <v>193</v>
       </c>
@@ -5156,7 +5153,7 @@
       <c r="J92" s="5"/>
       <c r="K92" s="9"/>
     </row>
-    <row r="93" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="29" t="s">
         <v>193</v>
       </c>
@@ -5178,7 +5175,7 @@
       <c r="J93" s="5"/>
       <c r="K93" s="9"/>
     </row>
-    <row r="94" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="29" t="s">
         <v>193</v>
       </c>
@@ -5202,7 +5199,7 @@
       <c r="J94" s="5"/>
       <c r="K94" s="9"/>
     </row>
-    <row r="95" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="29" t="s">
         <v>193</v>
       </c>
@@ -5224,7 +5221,7 @@
       <c r="J95" s="5"/>
       <c r="K95" s="9"/>
     </row>
-    <row r="96" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="29" t="s">
         <v>193</v>
       </c>
@@ -5248,7 +5245,7 @@
       <c r="J96" s="5"/>
       <c r="K96" s="9"/>
     </row>
-    <row r="97" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="29" t="s">
         <v>193</v>
       </c>
@@ -5266,7 +5263,7 @@
       <c r="J97" s="5"/>
       <c r="K97" s="9"/>
     </row>
-    <row r="98" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="29" t="s">
         <v>193</v>
       </c>
@@ -5288,7 +5285,7 @@
       <c r="J98" s="5"/>
       <c r="K98" s="9"/>
     </row>
-    <row r="99" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="29" t="s">
         <v>193</v>
       </c>
@@ -5312,7 +5309,7 @@
       <c r="J99" s="5"/>
       <c r="K99" s="9"/>
     </row>
-    <row r="100" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="29" t="s">
         <v>193</v>
       </c>
@@ -5334,7 +5331,7 @@
       <c r="J100" s="5"/>
       <c r="K100" s="9"/>
     </row>
-    <row r="101" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="29" t="s">
         <v>193</v>
       </c>
@@ -5358,7 +5355,7 @@
       <c r="J101" s="5"/>
       <c r="K101" s="9"/>
     </row>
-    <row r="102" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="29" t="s">
         <v>193</v>
       </c>
@@ -5376,7 +5373,7 @@
       <c r="J102" s="5"/>
       <c r="K102" s="9"/>
     </row>
-    <row r="103" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="29" t="s">
         <v>193</v>
       </c>
@@ -5398,7 +5395,7 @@
       <c r="J103" s="5"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="29" t="s">
         <v>193</v>
       </c>
@@ -5422,7 +5419,7 @@
       <c r="J104" s="5"/>
       <c r="K104" s="9"/>
     </row>
-    <row r="105" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="29" t="s">
         <v>193</v>
       </c>
@@ -5444,7 +5441,7 @@
       <c r="J105" s="5"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="29" t="s">
         <v>193</v>
       </c>
@@ -5464,7 +5461,7 @@
       <c r="J106" s="5"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="29" t="s">
         <v>193</v>
       </c>
@@ -5490,7 +5487,7 @@
       <c r="J107" s="5"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="29" t="s">
         <v>193</v>
       </c>
@@ -5514,7 +5511,7 @@
       <c r="J108" s="5"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="29" t="s">
         <v>193</v>
       </c>
@@ -5536,7 +5533,7 @@
       <c r="J109" s="5"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="29" t="s">
         <v>193</v>
       </c>
@@ -5556,7 +5553,7 @@
       <c r="J110" s="5"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="29" t="s">
         <v>193</v>
       </c>
@@ -5576,7 +5573,7 @@
       <c r="J111" s="5"/>
       <c r="K111" s="9"/>
     </row>
-    <row r="112" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="29" t="s">
         <v>193</v>
       </c>
@@ -5604,7 +5601,7 @@
       <c r="J112" s="5"/>
       <c r="K112" s="9"/>
     </row>
-    <row r="113" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="29" t="s">
         <v>193</v>
       </c>
@@ -5626,7 +5623,7 @@
       <c r="J113" s="5"/>
       <c r="K113" s="9"/>
     </row>
-    <row r="114" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="29" t="s">
         <v>193</v>
       </c>
@@ -5648,7 +5645,7 @@
       <c r="J114" s="5"/>
       <c r="K114" s="9"/>
     </row>
-    <row r="115" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="29" t="s">
         <v>193</v>
       </c>
@@ -5672,7 +5669,7 @@
       <c r="J115" s="5"/>
       <c r="K115" s="9"/>
     </row>
-    <row r="116" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="29" t="s">
         <v>193</v>
       </c>
@@ -5694,7 +5691,7 @@
       <c r="J116" s="5"/>
       <c r="K116" s="9"/>
     </row>
-    <row r="117" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="29" t="s">
         <v>193</v>
       </c>
@@ -5718,7 +5715,7 @@
       <c r="J117" s="5"/>
       <c r="K117" s="9"/>
     </row>
-    <row r="118" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="29" t="s">
         <v>193</v>
       </c>
@@ -5742,7 +5739,7 @@
       <c r="J118" s="5"/>
       <c r="K118" s="9"/>
     </row>
-    <row r="119" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="29" t="s">
         <v>193</v>
       </c>
@@ -5764,7 +5761,7 @@
       <c r="J119" s="5"/>
       <c r="K119" s="9"/>
     </row>
-    <row r="120" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="29" t="s">
         <v>193</v>
       </c>
@@ -5782,7 +5779,7 @@
       <c r="J120" s="5"/>
       <c r="K120" s="9"/>
     </row>
-    <row r="121" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="29" t="s">
         <v>193</v>
       </c>
@@ -5790,7 +5787,7 @@
         <v>406</v>
       </c>
       <c r="D121" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E121" s="49" t="s">
         <v>183</v>
@@ -5808,7 +5805,7 @@
       <c r="J121" s="5"/>
       <c r="K121" s="9"/>
     </row>
-    <row r="122" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="29" t="s">
         <v>193</v>
       </c>
@@ -5830,7 +5827,7 @@
       <c r="J122" s="5"/>
       <c r="K122" s="9"/>
     </row>
-    <row r="123" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="29" t="s">
         <v>193</v>
       </c>
@@ -5852,7 +5849,7 @@
       <c r="J123" s="5"/>
       <c r="K123" s="9"/>
     </row>
-    <row r="124" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="29" t="s">
         <v>193</v>
       </c>
@@ -5876,7 +5873,7 @@
       <c r="J124" s="5"/>
       <c r="K124" s="9"/>
     </row>
-    <row r="125" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="29" t="s">
         <v>193</v>
       </c>
@@ -5898,7 +5895,7 @@
       <c r="J125" s="5"/>
       <c r="K125" s="9"/>
     </row>
-    <row r="126" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="29" t="s">
         <v>193</v>
       </c>
@@ -5922,7 +5919,7 @@
       <c r="J126" s="5"/>
       <c r="K126" s="9"/>
     </row>
-    <row r="127" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="29" t="s">
         <v>193</v>
       </c>
@@ -5942,7 +5939,7 @@
       <c r="J127" s="5"/>
       <c r="K127" s="9"/>
     </row>
-    <row r="128" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="36" t="s">
         <v>193</v>
       </c>
@@ -5964,7 +5961,7 @@
       <c r="J128" s="5"/>
       <c r="K128" s="9"/>
     </row>
-    <row r="129" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="22" t="s">
         <v>18</v>
       </c>
@@ -5986,7 +5983,7 @@
       <c r="J129" s="5"/>
       <c r="K129" s="9"/>
     </row>
-    <row r="130" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="29" t="s">
         <v>18</v>
       </c>
@@ -6010,7 +6007,7 @@
       <c r="J130" s="5"/>
       <c r="K130" s="9"/>
     </row>
-    <row r="131" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B131" s="47" t="s">
         <v>18</v>
       </c>
@@ -6018,7 +6015,7 @@
         <v>226</v>
       </c>
       <c r="D131" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E131" s="49" t="s">
         <v>183</v>
@@ -6036,7 +6033,7 @@
       <c r="J131" s="5"/>
       <c r="K131" s="9"/>
     </row>
-    <row r="132" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="29" t="s">
         <v>18</v>
       </c>
@@ -6058,7 +6055,7 @@
       <c r="J132" s="5"/>
       <c r="K132" s="9"/>
     </row>
-    <row r="133" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="29" t="s">
         <v>18</v>
       </c>
@@ -6082,7 +6079,7 @@
       <c r="J133" s="5"/>
       <c r="K133" s="9"/>
     </row>
-    <row r="134" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="47" t="s">
         <v>18</v>
       </c>
@@ -6090,7 +6087,7 @@
         <v>229</v>
       </c>
       <c r="D134" s="48" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E134" s="49" t="s">
         <v>183</v>
@@ -6108,7 +6105,7 @@
       <c r="J134" s="5"/>
       <c r="K134" s="9"/>
     </row>
-    <row r="135" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="29" t="s">
         <v>18</v>
       </c>
@@ -6128,7 +6125,7 @@
       <c r="J135" s="5"/>
       <c r="K135" s="9"/>
     </row>
-    <row r="136" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="29" t="s">
         <v>18</v>
       </c>
@@ -6148,7 +6145,7 @@
       <c r="J136" s="5"/>
       <c r="K136" s="9"/>
     </row>
-    <row r="137" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="29" t="s">
         <v>18</v>
       </c>
@@ -6170,7 +6167,7 @@
       <c r="J137" s="5"/>
       <c r="K137" s="9"/>
     </row>
-    <row r="138" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B138" s="29" t="s">
         <v>18</v>
       </c>
@@ -6190,7 +6187,7 @@
       <c r="J138" s="5"/>
       <c r="K138" s="9"/>
     </row>
-    <row r="139" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="29" t="s">
         <v>18</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>573</v>
       </c>
       <c r="D139" s="30" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E139" s="31" t="s">
         <v>361</v>
@@ -6212,7 +6209,7 @@
       <c r="J139" s="5"/>
       <c r="K139" s="9"/>
     </row>
-    <row r="140" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="29" t="s">
         <v>18</v>
       </c>
@@ -6232,7 +6229,7 @@
       <c r="J140" s="5"/>
       <c r="K140" s="9"/>
     </row>
-    <row r="141" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="29" t="s">
         <v>18</v>
       </c>
@@ -6252,7 +6249,7 @@
       <c r="J141" s="5"/>
       <c r="K141" s="9"/>
     </row>
-    <row r="142" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="29" t="s">
         <v>18</v>
       </c>
@@ -6272,7 +6269,7 @@
       <c r="J142" s="5"/>
       <c r="K142" s="9"/>
     </row>
-    <row r="143" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="29" t="s">
         <v>18</v>
       </c>
@@ -6292,7 +6289,7 @@
       <c r="J143" s="5"/>
       <c r="K143" s="9"/>
     </row>
-    <row r="144" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="29" t="s">
         <v>18</v>
       </c>
@@ -6312,7 +6309,7 @@
       <c r="J144" s="5"/>
       <c r="K144" s="9"/>
     </row>
-    <row r="145" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="29" t="s">
         <v>18</v>
       </c>
@@ -6332,7 +6329,7 @@
       <c r="J145" s="5"/>
       <c r="K145" s="9"/>
     </row>
-    <row r="146" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="29" t="s">
         <v>18</v>
       </c>
@@ -6352,7 +6349,7 @@
       <c r="J146" s="5"/>
       <c r="K146" s="9"/>
     </row>
-    <row r="147" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="29" t="s">
         <v>18</v>
       </c>
@@ -6372,7 +6369,7 @@
       <c r="J147" s="5"/>
       <c r="K147" s="9"/>
     </row>
-    <row r="148" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="47" t="s">
         <v>18</v>
       </c>
@@ -6392,7 +6389,7 @@
       <c r="J148" s="5"/>
       <c r="K148" s="9"/>
     </row>
-    <row r="149" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="47" t="s">
         <v>18</v>
       </c>
@@ -6412,7 +6409,7 @@
       <c r="J149" s="5"/>
       <c r="K149" s="9"/>
     </row>
-    <row r="150" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="47" t="s">
         <v>18</v>
       </c>
@@ -6432,7 +6429,7 @@
       <c r="J150" s="5"/>
       <c r="K150" s="9"/>
     </row>
-    <row r="151" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B151" s="47" t="s">
         <v>18</v>
       </c>
@@ -6452,7 +6449,7 @@
       <c r="J151" s="5"/>
       <c r="K151" s="9"/>
     </row>
-    <row r="152" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B152" s="47" t="s">
         <v>18</v>
       </c>
@@ -6472,7 +6469,7 @@
       <c r="J152" s="5"/>
       <c r="K152" s="9"/>
     </row>
-    <row r="153" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="47" t="s">
         <v>18</v>
       </c>
@@ -6492,7 +6489,7 @@
       <c r="J153" s="5"/>
       <c r="K153" s="9"/>
     </row>
-    <row r="154" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="47" t="s">
         <v>18</v>
       </c>
@@ -6512,7 +6509,7 @@
       <c r="J154" s="5"/>
       <c r="K154" s="9"/>
     </row>
-    <row r="155" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="56" t="s">
         <v>18</v>
       </c>
@@ -6532,7 +6529,7 @@
       <c r="J155" s="5"/>
       <c r="K155" s="9"/>
     </row>
-    <row r="156" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B156" s="22" t="s">
         <v>27</v>
       </c>
@@ -6554,7 +6551,7 @@
       <c r="J156" s="5"/>
       <c r="K156" s="9"/>
     </row>
-    <row r="157" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="29" t="s">
         <v>27</v>
       </c>
@@ -6578,7 +6575,7 @@
       <c r="J157" s="5"/>
       <c r="K157" s="9"/>
     </row>
-    <row r="158" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B158" s="29" t="s">
         <v>27</v>
       </c>
@@ -6596,7 +6593,7 @@
       <c r="J158" s="5"/>
       <c r="K158" s="9"/>
     </row>
-    <row r="159" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="29" t="s">
         <v>27</v>
       </c>
@@ -6618,7 +6615,7 @@
       <c r="J159" s="5"/>
       <c r="K159" s="9"/>
     </row>
-    <row r="160" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B160" s="29" t="s">
         <v>27</v>
       </c>
@@ -6642,7 +6639,7 @@
       <c r="J160" s="5"/>
       <c r="K160" s="9"/>
     </row>
-    <row r="161" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B161" s="29" t="s">
         <v>27</v>
       </c>
@@ -6664,7 +6661,7 @@
       <c r="J161" s="5"/>
       <c r="K161" s="9"/>
     </row>
-    <row r="162" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B162" s="29" t="s">
         <v>27</v>
       </c>
@@ -6688,7 +6685,7 @@
       <c r="J162" s="5"/>
       <c r="K162" s="9"/>
     </row>
-    <row r="163" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B163" s="29" t="s">
         <v>27</v>
       </c>
@@ -6710,7 +6707,7 @@
       <c r="J163" s="5"/>
       <c r="K163" s="9"/>
     </row>
-    <row r="164" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="29" t="s">
         <v>27</v>
       </c>
@@ -6732,7 +6729,7 @@
       <c r="J164" s="5"/>
       <c r="K164" s="9"/>
     </row>
-    <row r="165" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B165" s="36" t="s">
         <v>27</v>
       </c>
@@ -6740,7 +6737,7 @@
         <v>175</v>
       </c>
       <c r="D165" s="57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E165" s="58" t="s">
         <v>183</v>
@@ -6758,7 +6755,7 @@
       <c r="J165" s="5"/>
       <c r="K165" s="9"/>
     </row>
-    <row r="166" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="22" t="s">
         <v>234</v>
       </c>
@@ -6780,7 +6777,7 @@
       <c r="J166" s="5"/>
       <c r="K166" s="9"/>
     </row>
-    <row r="167" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="29" t="s">
         <v>234</v>
       </c>
@@ -6800,7 +6797,7 @@
       <c r="J167" s="5"/>
       <c r="K167" s="9"/>
     </row>
-    <row r="168" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="29" t="s">
         <v>234</v>
       </c>
@@ -6820,7 +6817,7 @@
       <c r="J168" s="5"/>
       <c r="K168" s="9"/>
     </row>
-    <row r="169" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="29" t="s">
         <v>234</v>
       </c>
@@ -6840,7 +6837,7 @@
       <c r="J169" s="5"/>
       <c r="K169" s="9"/>
     </row>
-    <row r="170" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="29" t="s">
         <v>234</v>
       </c>
@@ -6860,7 +6857,7 @@
       <c r="J170" s="5"/>
       <c r="K170" s="9"/>
     </row>
-    <row r="171" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B171" s="29" t="s">
         <v>234</v>
       </c>
@@ -6880,7 +6877,7 @@
       <c r="J171" s="5"/>
       <c r="K171" s="9"/>
     </row>
-    <row r="172" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B172" s="29" t="s">
         <v>234</v>
       </c>
@@ -6900,7 +6897,7 @@
       <c r="J172" s="5"/>
       <c r="K172" s="9"/>
     </row>
-    <row r="173" spans="2:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B173" s="47" t="s">
         <v>234</v>
       </c>
@@ -6920,7 +6917,7 @@
       <c r="J173" s="13"/>
       <c r="K173" s="14"/>
     </row>
-    <row r="174" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B174" s="29" t="s">
         <v>234</v>
       </c>
@@ -6940,7 +6937,7 @@
       <c r="J174" s="5"/>
       <c r="K174" s="9"/>
     </row>
-    <row r="175" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B175" s="29" t="s">
         <v>234</v>
       </c>
@@ -6948,7 +6945,7 @@
         <v>248</v>
       </c>
       <c r="D175" s="30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E175" s="31" t="s">
         <v>251</v>
@@ -6962,7 +6959,7 @@
       <c r="J175" s="5"/>
       <c r="K175" s="9"/>
     </row>
-    <row r="176" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="29" t="s">
         <v>234</v>
       </c>
@@ -6982,7 +6979,7 @@
       <c r="J176" s="5"/>
       <c r="K176" s="9"/>
     </row>
-    <row r="177" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="29" t="s">
         <v>234</v>
       </c>
@@ -7002,7 +6999,7 @@
       <c r="J177" s="5"/>
       <c r="K177" s="9"/>
     </row>
-    <row r="178" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="29" t="s">
         <v>234</v>
       </c>
@@ -7022,7 +7019,7 @@
       <c r="J178" s="5"/>
       <c r="K178" s="9"/>
     </row>
-    <row r="179" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="36" t="s">
         <v>234</v>
       </c>
@@ -7042,7 +7039,7 @@
       <c r="J179" s="5"/>
       <c r="K179" s="9"/>
     </row>
-    <row r="180" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B180" s="22" t="s">
         <v>123</v>
       </c>
@@ -7066,7 +7063,7 @@
       <c r="J180" s="5"/>
       <c r="K180" s="9"/>
     </row>
-    <row r="181" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B181" s="29" t="s">
         <v>123</v>
       </c>
@@ -7088,7 +7085,7 @@
       <c r="J181" s="5"/>
       <c r="K181" s="9"/>
     </row>
-    <row r="182" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B182" s="29" t="s">
         <v>123</v>
       </c>
@@ -7110,7 +7107,7 @@
       <c r="J182" s="5"/>
       <c r="K182" s="9"/>
     </row>
-    <row r="183" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="29" t="s">
         <v>123</v>
       </c>
@@ -7134,7 +7131,7 @@
       <c r="J183" s="5"/>
       <c r="K183" s="9"/>
     </row>
-    <row r="184" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B184" s="68" t="s">
         <v>123</v>
       </c>
@@ -7142,7 +7139,7 @@
         <v>176</v>
       </c>
       <c r="D184" s="69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E184" s="70" t="s">
         <v>183</v>
@@ -7160,7 +7157,7 @@
       <c r="J184" s="5"/>
       <c r="K184" s="9"/>
     </row>
-    <row r="185" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
@@ -7171,9 +7168,9 @@
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
     </row>
-    <row r="186" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B186" s="78" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C186" s="78"/>
       <c r="D186" s="78"/>
@@ -7184,7 +7181,7 @@
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
     </row>
-    <row r="187" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
@@ -7201,7 +7198,7 @@
     <hyperlink ref="C4" r:id="rId1" display="https://ason.ch/api/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="27" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="26" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"-,Bold"Payroll Engine&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>